<commit_message>
Atualizei os arquivos de dados do Supplementary Appendix A
</commit_message>
<xml_diff>
--- a/Artigo 4/Supplementary Appendix A/data_dictionary.xlsx
+++ b/Artigo 4/Supplementary Appendix A/data_dictionary.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27dfba7ba8e15536/Área de Trabalho/artigo_mortalidades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27dfba7ba8e15536/Área de Trabalho/Material_Suplementar/Artigo 4/Supplementary Appendix A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{E05B6A7C-979D-4F96-B4B1-DADAE3ED06F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF896B4E-ACC5-437B-A35D-4101044855F5}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{E05B6A7C-979D-4F96-B4B1-DADAE3ED06F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EBF08C3-1E7E-423D-935D-7F334B3FEB9B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8DACC71-C19B-4685-8031-FA35FFFBDCEF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8DACC71-C19B-4685-8031-FA35FFFBDCEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="Model Chronic" sheetId="2" r:id="rId2"/>
-    <sheet name="Boruta Chronic Model" sheetId="3" r:id="rId3"/>
+    <sheet name="Model Chronic General" sheetId="2" r:id="rId2"/>
+    <sheet name="Boruta Chronic Model - General" sheetId="3" r:id="rId3"/>
+    <sheet name="Boruta Chronic Model - 20,000" sheetId="4" r:id="rId4"/>
+    <sheet name="Boruta Chronic Model - 50,000" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Model Chronic'!$A$1:$C$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Model Chronic General'!$A$1:$C$120</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Total Variables'!$A$1:$C$284</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="381">
   <si>
     <t>Variable</t>
   </si>
@@ -1247,10 +1249,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1552,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37754E0-9C5B-4EE5-9433-D7345726A3A3}">
   <dimension ref="A1:C284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4698,7 +4696,7 @@
   <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6276,7 +6274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF6C97D-DF70-4EA2-9510-3EB265471452}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6301,11 +6301,11 @@
         <v>90</v>
       </c>
       <c r="B2" t="str">
-        <f>VLOOKUP(A2,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A2,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Average Income</v>
       </c>
       <c r="C2" t="str">
-        <f>VLOOKUP(A2,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A2,'Model Chronic General'!$A:$C,3,0)</f>
         <v>White</v>
       </c>
     </row>
@@ -6314,11 +6314,11 @@
         <v>93</v>
       </c>
       <c r="B3" t="str">
-        <f>VLOOKUP(A3,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Average Income</v>
       </c>
       <c r="C3" t="str">
-        <f>VLOOKUP(A3,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,3,0)</f>
         <v>Brown</v>
       </c>
     </row>
@@ -6327,11 +6327,11 @@
         <v>107</v>
       </c>
       <c r="B4" t="str">
-        <f>VLOOKUP(A4,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A4,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Social benefits for deficient population</v>
       </c>
       <c r="C4" t="str">
-        <f>VLOOKUP(A4,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A4,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6340,11 +6340,11 @@
         <v>108</v>
       </c>
       <c r="B5" t="str">
-        <f>VLOOKUP(A5,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A5,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Garbage collected by cleaning service</v>
       </c>
       <c r="C5" t="str">
-        <f>VLOOKUP(A5,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A5,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6353,11 +6353,11 @@
         <v>110</v>
       </c>
       <c r="B6" t="str">
-        <f>VLOOKUP(A6,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Garbage burned on the property</v>
       </c>
       <c r="C6" t="str">
-        <f>VLOOKUP(A6,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6366,11 +6366,11 @@
         <v>116</v>
       </c>
       <c r="B7" t="str">
-        <f>VLOOKUP(A7,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Demographic density</v>
       </c>
       <c r="C7" t="str">
-        <f>VLOOKUP(A7,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6379,11 +6379,11 @@
         <v>119</v>
       </c>
       <c r="B8" t="str">
-        <f>VLOOKUP(A8,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of urban population</v>
       </c>
       <c r="C8" t="str">
-        <f>VLOOKUP(A8,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,3,0)</f>
         <v>Urban Population</v>
       </c>
     </row>
@@ -6392,11 +6392,11 @@
         <v>137</v>
       </c>
       <c r="B9" t="str">
-        <f>VLOOKUP(A9,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A9,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Source of water distribution - sewer or pluvial network</v>
       </c>
       <c r="C9" t="str">
-        <f>VLOOKUP(A9,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A9,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6405,11 +6405,11 @@
         <v>145</v>
       </c>
       <c r="B10" t="str">
-        <f>VLOOKUP(A10,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A10,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of the population with twenty-five years and over with incomplete high school</v>
       </c>
       <c r="C10" t="str">
-        <f>VLOOKUP(A10,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A10,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6418,11 +6418,11 @@
         <v>163</v>
       </c>
       <c r="B11" t="str">
-        <f>VLOOKUP(A11,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A11,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Unemployment rate</v>
       </c>
       <c r="C11" t="str">
-        <f>VLOOKUP(A11,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A11,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6431,11 +6431,11 @@
         <v>313</v>
       </c>
       <c r="B12" t="str">
-        <f>VLOOKUP(A12,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A12,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of residence without surrounding afforestation</v>
       </c>
       <c r="C12" t="str">
-        <f>VLOOKUP(A12,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A12,'Model Chronic General'!$A:$C,3,0)</f>
         <v>White</v>
       </c>
     </row>
@@ -6444,11 +6444,11 @@
         <v>368</v>
       </c>
       <c r="B13" t="str">
-        <f>VLOOKUP(A13,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A13,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of population in both religious and civil marriage</v>
       </c>
       <c r="C13" t="str">
-        <f>VLOOKUP(A13,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A13,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6457,11 +6457,11 @@
         <v>370</v>
       </c>
       <c r="B14" t="str">
-        <f>VLOOKUP(A14,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A14,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of population in a civil marriage</v>
       </c>
       <c r="C14" t="str">
-        <f>VLOOKUP(A14,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A14,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6470,11 +6470,11 @@
         <v>371</v>
       </c>
       <c r="B15" t="str">
-        <f>VLOOKUP(A15,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A15,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Percent of population in a consensual union</v>
       </c>
       <c r="C15" t="str">
-        <f>VLOOKUP(A15,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A15,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6483,11 +6483,11 @@
         <v>115</v>
       </c>
       <c r="B16" t="str">
-        <f>VLOOKUP(A16,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A16,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Gross domestic product (GDP) per capita</v>
       </c>
       <c r="C16" t="str">
-        <f>VLOOKUP(A16,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A16,'Model Chronic General'!$A:$C,3,0)</f>
         <v>General</v>
       </c>
     </row>
@@ -6496,12 +6496,244 @@
         <v>174</v>
       </c>
       <c r="B17" t="str">
-        <f>VLOOKUP(A17,'Model Chronic'!$A:$C,2,0)</f>
+        <f>VLOOKUP(A17,'Model Chronic General'!$A:$C,2,0)</f>
         <v>Illiteracy Rate</v>
       </c>
       <c r="C17" t="str">
-        <f>VLOOKUP(A17,'Model Chronic'!$A:$C,3,0)</f>
+        <f>VLOOKUP(A17,'Model Chronic General'!$A:$C,3,0)</f>
         <v>Black</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9867E1AD-5FD2-404C-A531-CF97260621AE}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Source of water distribution - sewer or pluvial network</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Percent of population in both religious and civil marriage</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Percent of population in a consensual union</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Demographic density</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A12F77-530C-42E9-9116-E062B6EFCF13}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Source of water distribution - sewer or pluvial network</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(A3,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Percent of population in both religious and civil marriage</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(A6,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Percent of population in a consensual union</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(A7,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,2,0)</f>
+        <v>Demographic density</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(A8,'Model Chronic General'!$A:$C,3,0)</f>
+        <v>General</v>
       </c>
     </row>
   </sheetData>

</xml_diff>